<commit_message>
Mise en place de sac à dos simple, illimités et multiples en excel et python
</commit_message>
<xml_diff>
--- a/26. Recherche opérationnelle en Excel/40 - SAC A DOS SIMPLE - EXCEL/01. KnapSack 0-1 en Français.xlsx
+++ b/26. Recherche opérationnelle en Excel/40 - SAC A DOS SIMPLE - EXCEL/01. KnapSack 0-1 en Français.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\www\python-data-science2\26. Recherche opérationnelle en Excel\40 - KNAPSAC SIMPLE - EXCEL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\www\python-data-science2\26. Recherche opérationnelle en Excel\40 - SAC A DOS SIMPLE - EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -233,6 +233,93 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5699760" cy="3086100"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4579620" y="2491740"/>
+          <a:ext cx="5699760" cy="3086100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>265746</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>496341</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>174308</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4532946" y="2179320"/>
+          <a:ext cx="5716995" cy="4944428"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -501,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:L10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>